<commit_message>
excel sheets modified, line delete button added
</commit_message>
<xml_diff>
--- a/backend/templates/102-18c-white.xlsx
+++ b/backend/templates/102-18c-white.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cursor AI Projects\SwansonIndiaPortal\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56043199-FE7A-494D-8A88-BA8AC0808F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9028A1F-06D2-4983-A386-248EDB65E9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="637" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,11 +522,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000_ "/>
     <numFmt numFmtId="167" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="169" formatCode="[$-14009]dd\-mm\-yyyy;@"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -2329,7 +2330,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -8539,12 +8540,12 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>

</xml_diff>